<commit_message>
Finished parsing penn data and added VS code support via poetry toml
</commit_message>
<xml_diff>
--- a/datparser/raw_inputs/pennington_feasibility/misc_data.xlsx
+++ b/datparser/raw_inputs/pennington_feasibility/misc_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/94f8da091d404851/Documents/Masters/Misc/phi_kappa_psi/HC/new_property/misc/alumni_data/datparser/raw_inputs/pennington_feasibility/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOS\PERSONAL\pkp_alumni_data\datparser\raw_inputs\pennington_feasibility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E87DCAC-E909-40BD-9F6C-06DE3A49058F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104503D3-FEEE-471D-80C4-4F6C85081BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26D654B0-E92D-4502-BDA3-55B09334B842}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26D654B0-E92D-4502-BDA3-55B09334B842}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -49,9 +48,6 @@
     <t>arjpaz@gmail.com</t>
   </si>
   <si>
-    <t>Notes say have Butch reach out, otherwise Jeff</t>
-  </si>
-  <si>
     <t>1975's</t>
   </si>
   <si>
@@ -338,6 +334,9 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Notes say have Butch reach out otherwise Jeff</t>
   </si>
 </sst>
 </file>
@@ -692,53 +691,53 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>84</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>86</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>87</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>88</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>89</v>
       </c>
-      <c r="M1" t="s">
-        <v>90</v>
-      </c>
       <c r="N1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -758,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="N2" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -766,16 +765,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="N3" t="s">
         <v>7</v>
-      </c>
-      <c r="N3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -783,19 +782,19 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="L4" t="s">
         <v>11</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>12</v>
-      </c>
-      <c r="N4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -803,16 +802,16 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -820,19 +819,19 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="L6" t="s">
         <v>16</v>
       </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
       <c r="N6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -840,16 +839,16 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="N7" t="s">
         <v>20</v>
-      </c>
-      <c r="N7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -857,16 +856,16 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
       <c r="N8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -874,19 +873,19 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="L9" t="s">
         <v>25</v>
       </c>
-      <c r="L9" t="s">
-        <v>26</v>
-      </c>
       <c r="N9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -894,19 +893,19 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
+      <c r="L10" t="s">
         <v>29</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>30</v>
-      </c>
-      <c r="N10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -914,22 +913,22 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="J11" t="s">
         <v>33</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>34</v>
       </c>
-      <c r="L11" t="s">
-        <v>35</v>
-      </c>
       <c r="N11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -937,16 +936,16 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
-        <v>37</v>
-      </c>
       <c r="N12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -954,22 +953,22 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
+      <c r="J13" t="s">
         <v>40</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>41</v>
       </c>
-      <c r="L13" t="s">
-        <v>42</v>
-      </c>
       <c r="N13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -977,16 +976,16 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
       <c r="N14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -994,22 +993,22 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s">
+      <c r="J15" t="s">
         <v>47</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>48</v>
       </c>
-      <c r="L15" t="s">
-        <v>49</v>
-      </c>
       <c r="N15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1017,19 +1016,19 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
         <v>50</v>
       </c>
-      <c r="D16" t="s">
+      <c r="L16" t="s">
         <v>51</v>
       </c>
-      <c r="L16" t="s">
-        <v>52</v>
-      </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1037,22 +1036,22 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
+      <c r="J17" t="s">
         <v>54</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>55</v>
       </c>
-      <c r="L17" t="s">
-        <v>56</v>
-      </c>
       <c r="N17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1060,16 +1059,16 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
-        <v>58</v>
-      </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1077,19 +1076,19 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
         <v>59</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>60</v>
       </c>
-      <c r="D19" t="s">
+      <c r="L19" t="s">
         <v>61</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>62</v>
-      </c>
-      <c r="N19" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1097,19 +1096,19 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
         <v>64</v>
       </c>
-      <c r="D20" t="s">
+      <c r="L20" t="s">
         <v>65</v>
       </c>
-      <c r="L20" t="s">
-        <v>66</v>
-      </c>
       <c r="N20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1117,68 +1116,68 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
         <v>67</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>68</v>
       </c>
-      <c r="D21" t="s">
+      <c r="J21" t="s">
         <v>69</v>
       </c>
-      <c r="J21" t="s">
+      <c r="L21" t="s">
         <v>70</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>71</v>
-      </c>
-      <c r="N21" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22">
         <v>1975</v>
       </c>
       <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
         <v>74</v>
       </c>
-      <c r="D22" t="s">
+      <c r="L22" t="s">
         <v>75</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>76</v>
-      </c>
-      <c r="N22" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
         <v>95</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>96</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>97</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" t="s">
         <v>98</v>
       </c>
-      <c r="F27" t="s">
-        <v>78</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>99</v>
-      </c>
-      <c r="H27" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -1186,19 +1185,19 @@
         <v>2000</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>